<commit_message>
Update 2.38 Chrome Driver
</commit_message>
<xml_diff>
--- a/MavenHybridDataDriven/data/login.xlsx
+++ b/MavenHybridDataDriven/data/login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5ABD5102-8353-480E-9C00-FB9029134AFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0A37CC62-0EA0-4856-8F7B-A355F46C2E6F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Account title</t>
+  </si>
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>Initial balance</t>
+  </si>
+  <si>
+    <t>saving</t>
+  </si>
+  <si>
     <t>techfiosdemo@gmail.com</t>
   </si>
   <si>
@@ -32,82 +47,94 @@
     <t>Name</t>
   </si>
   <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Sale Price</t>
+  </si>
+  <si>
+    <t>Itemnumber</t>
+  </si>
+  <si>
+    <t>Ac10</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
     <t>company</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
+    <t>phone</t>
+  </si>
+  <si>
     <t>address</t>
   </si>
   <si>
+    <t>state</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>zip</t>
   </si>
   <si>
+    <t>Hp</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Descrption</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Tution</t>
+  </si>
+  <si>
+    <t>Account Info</t>
+  </si>
+  <si>
+    <t>School Fund</t>
+  </si>
+  <si>
+    <t>Belalsavings</t>
+  </si>
+  <si>
+    <t>Mohammed Rashid</t>
+  </si>
+  <si>
     <t>rashid@gmail.com</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>itemnumber</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>belal</t>
-  </si>
-  <si>
-    <t>ac10</t>
-  </si>
-  <si>
-    <t>butter</t>
-  </si>
-  <si>
-    <t>techfiosbilling</t>
-  </si>
-  <si>
-    <t>xyz company</t>
-  </si>
-  <si>
-    <t>123 irving</t>
-  </si>
-  <si>
-    <t>irving</t>
-  </si>
-  <si>
-    <t>tx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">account </t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Accounttitle</t>
-  </si>
-  <si>
-    <t>initialbalance</t>
+    <t>2484806055</t>
+  </si>
+  <si>
+    <t>123 Irving</t>
+  </si>
+  <si>
+    <t>Irving</t>
+  </si>
+  <si>
+    <t>75062</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,27 +173,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,147 +521,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1"/>
-    <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="16" width="8.7109375" style="1"/>
-    <col min="17" max="17" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="6">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="7">
-        <v>2484806055</v>
+        <v>31</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="7">
-        <v>75062</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M5" s="3"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M7" s="3"/>
+      <c r="Q2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="5">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>